<commit_message>
UT clean up to xlsx files
</commit_message>
<xml_diff>
--- a/InputData/bldgs/BFoCSbQL/BAU Frac of Components Sold by Quality Lvl.xlsx
+++ b/InputData/bldgs/BFoCSbQL/BAU Frac of Components Sold by Quality Lvl.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Dropbox (Energy Innovation)\EPS Documents\Regional Adaptation Work\Texas\Texas EPS\InputData\bldgs\BFoCSbQL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cmr4337\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="23880" yWindow="-120" windowWidth="29040" windowHeight="17640"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="BFoCSbQL-rural-residential" sheetId="5" r:id="rId5"/>
     <sheet name="BFoCSbQL-commercial" sheetId="4" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -279,33 +279,15 @@
     <t>for energy efficient rebates.</t>
   </si>
   <si>
-    <t>So, this is basically an estimation of what hardware components of different appliances are</t>
-  </si>
-  <si>
-    <t xml:space="preserve">eligible for an energy start rebate. </t>
-  </si>
-  <si>
-    <t>Their method makes sense to me. They take a weighted average of the sales of different appliance components</t>
-  </si>
-  <si>
     <t>multiplied by the percentage of those components that qualify for an energy star rebate.</t>
   </si>
   <si>
-    <t>The data source they use (the Building Energy Data Book) might be a bit dated (2011)</t>
-  </si>
-  <si>
     <t>The only Texas specific data it has is that 43% of new houses in Texas are energy star qualified (vs. 24% for the rest of the US.)</t>
   </si>
   <si>
     <t>but I’m not sure if that translates to the other numbers being used in this study.</t>
   </si>
   <si>
-    <t>One change I did make</t>
-  </si>
-  <si>
-    <t>I removed oil boilers, oil furnaces, and gas furnaces from the calculations for the heating sector</t>
-  </si>
-  <si>
     <t>since those technologies are really uncommon in Texas</t>
   </si>
   <si>
@@ -321,7 +303,25 @@
     <t>in the residential sector, Texas natural gas is not used for boilers</t>
   </si>
   <si>
-    <t>wasn't able to find newer data on %energy star market share, though I suspect it is higher than it was in 2011.</t>
+    <t>Explanation</t>
+  </si>
+  <si>
+    <t>Changes from US to Texas</t>
+  </si>
+  <si>
+    <t>Removed oil boilers, oil furnaces, and gas furnaces from the calculations for the heating sector</t>
+  </si>
+  <si>
+    <t>**wasn't able to find newer data on %energy star market share.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is basically an estimation of what hardware components of different appliances are eligible for an energy start rebate. </t>
+  </si>
+  <si>
+    <t>This sheet takes a weighted average of the sales of different appliance components</t>
+  </si>
+  <si>
+    <t>The data source used (the Building Energy Data Book) might be a bit dated (2011)</t>
   </si>
 </sst>
 </file>
@@ -756,22 +756,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.73046875" customWidth="1"/>
-    <col min="2" max="2" width="54.265625" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="54.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -779,52 +779,52 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" s="2">
         <v>2012</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" s="6" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>77</v>
       </c>
@@ -843,42 +843,42 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26" customWidth="1"/>
     <col min="2" max="2" width="31" customWidth="1"/>
-    <col min="3" max="3" width="23.86328125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="24.265625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="18.73046875" customWidth="1"/>
-    <col min="6" max="6" width="59.86328125" customWidth="1"/>
+    <col min="3" max="3" width="23.85546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="24.28515625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" customWidth="1"/>
+    <col min="6" max="6" width="59.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
@@ -898,7 +898,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>66</v>
       </c>
@@ -918,7 +918,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>16</v>
       </c>
@@ -935,7 +935,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>17</v>
       </c>
@@ -952,7 +952,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
       <c r="B11" s="7" t="s">
         <v>18</v>
@@ -970,7 +970,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>65</v>
       </c>
@@ -990,7 +990,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="12" t="s">
         <v>13</v>
@@ -1008,7 +1008,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
       <c r="B14" s="7" t="s">
         <v>14</v>
@@ -1026,7 +1026,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>2</v>
       </c>
@@ -1046,7 +1046,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>37</v>
       </c>
@@ -1067,7 +1067,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>27</v>
       </c>
@@ -1085,7 +1085,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>28</v>
       </c>
@@ -1103,7 +1103,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>38</v>
       </c>
@@ -1123,7 +1123,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>34</v>
       </c>
@@ -1140,7 +1140,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>36</v>
       </c>
@@ -1157,7 +1157,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>40</v>
       </c>
@@ -1174,7 +1174,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>41</v>
       </c>
@@ -1191,7 +1191,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>42</v>
       </c>
@@ -1208,7 +1208,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>33</v>
       </c>
@@ -1225,7 +1225,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="7"/>
       <c r="B26" s="7" t="s">
         <v>35</v>
@@ -1243,7 +1243,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>43</v>
       </c>
@@ -1263,7 +1263,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>45</v>
       </c>
@@ -1280,7 +1280,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>46</v>
       </c>
@@ -1297,7 +1297,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>47</v>
       </c>
@@ -1314,7 +1314,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>48</v>
       </c>
@@ -1331,7 +1331,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -1352,7 +1352,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>56</v>
       </c>
@@ -1370,7 +1370,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>57</v>
       </c>
@@ -1388,7 +1388,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>58</v>
       </c>
@@ -1406,7 +1406,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>59</v>
       </c>
@@ -1424,7 +1424,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>60</v>
       </c>
@@ -1442,7 +1442,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>61</v>
       </c>
@@ -1491,94 +1491,98 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
+      <c r="C12" s="4" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A13" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B14" t="s">
-        <v>91</v>
-      </c>
-      <c r="C14" s="4" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B15" t="s">
-        <v>93</v>
-      </c>
       <c r="C15" s="4"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B16" t="s">
-        <v>94</v>
-      </c>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C16" s="4"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C17" s="4"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A18" t="s">
-        <v>95</v>
-      </c>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C18" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C14" r:id="rId1" location="building-characteristics" display="https://resstock.nrel.gov/dataviewer/efs_v2_base - building-characteristics"/>
+    <hyperlink ref="C12" r:id="rId1" location="building-characteristics" display="https://resstock.nrel.gov/dataviewer/efs_v2_base - building-characteristics"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1595,14 +1599,14 @@
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.86328125" customWidth="1"/>
-    <col min="2" max="2" width="20.86328125" customWidth="1"/>
+    <col min="1" max="1" width="28.85546875" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" customWidth="1"/>
     <col min="3" max="3" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>78</v>
       </c>
@@ -1613,7 +1617,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>66</v>
       </c>
@@ -1626,7 +1630,7 @@
         <v>0.61</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>65</v>
       </c>
@@ -1639,7 +1643,7 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>67</v>
       </c>
@@ -1652,7 +1656,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1665,7 +1669,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -1678,7 +1682,7 @@
         <v>0.67017241379310344</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -1709,14 +1713,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.86328125" customWidth="1"/>
-    <col min="2" max="2" width="20.86328125" customWidth="1"/>
+    <col min="1" max="1" width="28.85546875" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" customWidth="1"/>
     <col min="3" max="3" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>78</v>
       </c>
@@ -1727,7 +1731,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>66</v>
       </c>
@@ -1740,7 +1744,7 @@
         <v>0.61</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>65</v>
       </c>
@@ -1753,7 +1757,7 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>67</v>
       </c>
@@ -1766,7 +1770,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1779,7 +1783,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -1792,7 +1796,7 @@
         <v>0.67017241379310344</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -1820,14 +1824,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.86328125" customWidth="1"/>
-    <col min="2" max="2" width="20.86328125" customWidth="1"/>
+    <col min="1" max="1" width="28.85546875" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" customWidth="1"/>
     <col min="3" max="3" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>78</v>
       </c>
@@ -1838,7 +1842,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>66</v>
       </c>
@@ -1851,7 +1855,7 @@
         <v>0.61</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>65</v>
       </c>
@@ -1864,7 +1868,7 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>67</v>
       </c>
@@ -1877,7 +1881,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1890,7 +1894,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -1903,7 +1907,7 @@
         <v>0.46288946910356832</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>

</xml_diff>